<commit_message>
ödev 2 not güncellemesi
</commit_message>
<xml_diff>
--- a/notlar.xlsx
+++ b/notlar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet\Desktop\workspace\Algorithms-and-Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.kasif\Desktop\workspace\Algorithms-and-Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Öğrenci No</t>
   </si>
@@ -204,14 +204,14 @@
     <t>8) Ortak çözüm</t>
   </si>
   <si>
-    <t>Sürüm 1.0.0</t>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -263,6 +263,13 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -636,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -666,12 +673,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -732,9 +733,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,6 +749,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1059,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1074,10 +1099,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1101,22 +1126,22 @@
       <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5">
         <v>100</v>
       </c>
       <c r="D2" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -1133,23 +1158,23 @@
       <c r="I2" s="7">
         <v>0</v>
       </c>
-      <c r="J2" s="28">
+      <c r="J2" s="26">
         <f t="shared" ref="J2:J12" si="0">SUM(AVERAGE(C2:G2)/2,AVERAGE(H2:I2)/2)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="8">
         <v>100</v>
       </c>
       <c r="D3" s="9">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E3" s="9">
         <v>0</v>
@@ -1166,16 +1191,16 @@
       <c r="I3" s="10">
         <v>0</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8">
@@ -1199,23 +1224,23 @@
       <c r="I4" s="10">
         <v>0</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="27">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="8">
         <v>90</v>
       </c>
       <c r="D5" s="9">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E5" s="9">
         <v>0</v>
@@ -1232,23 +1257,23 @@
       <c r="I5" s="10">
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="27">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="8">
         <v>100</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -1265,23 +1290,23 @@
       <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="8">
         <v>90</v>
       </c>
       <c r="D7" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7" s="9">
         <v>0</v>
@@ -1298,23 +1323,23 @@
       <c r="I7" s="10">
         <v>0</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="27">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="8">
         <v>100</v>
       </c>
       <c r="D8" s="9">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="E8" s="9">
         <v>0</v>
@@ -1331,56 +1356,55 @@
       <c r="I8" s="10">
         <v>0</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8">
-        <v>100</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="10">
-        <v>0</v>
-      </c>
-      <c r="J9" s="29">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="C9" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="8">
         <v>60</v>
       </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
@@ -1397,23 +1421,23 @@
       <c r="I10" s="10">
         <v>0</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="27">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="8">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E11" s="9">
         <v>0</v>
@@ -1430,23 +1454,23 @@
       <c r="I11" s="10">
         <v>0</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="27">
         <f t="shared" si="0"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="8">
         <v>100</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E12" s="9">
         <v>0</v>
@@ -1463,23 +1487,23 @@
       <c r="I12" s="10">
         <v>0</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="8">
         <v>90</v>
       </c>
       <c r="D13" s="9">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E13" s="9">
         <v>0</v>
@@ -1496,23 +1520,23 @@
       <c r="I13" s="10">
         <v>0</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="27">
         <f t="shared" ref="J13:J21" si="1">SUM(AVERAGE(C13:G13)/2,AVERAGE(H13:I13)/2)</f>
-        <v>9</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="8">
         <v>100</v>
       </c>
       <c r="D14" s="9">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E14" s="9">
         <v>0</v>
@@ -1529,23 +1553,23 @@
       <c r="I14" s="10">
         <v>0</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="27">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="8">
         <v>100</v>
       </c>
       <c r="D15" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E15" s="9">
         <v>0</v>
@@ -1562,23 +1586,23 @@
       <c r="I15" s="10">
         <v>0</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="27">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="8">
         <v>100</v>
       </c>
       <c r="D16" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E16" s="9">
         <v>0</v>
@@ -1595,23 +1619,23 @@
       <c r="I16" s="10">
         <v>0</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="27">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="8">
         <v>90</v>
       </c>
       <c r="D17" s="9">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E17" s="9">
         <v>0</v>
@@ -1628,23 +1652,23 @@
       <c r="I17" s="10">
         <v>0</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="27">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="8">
         <v>100</v>
       </c>
       <c r="D18" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E18" s="9">
         <v>0</v>
@@ -1661,294 +1685,291 @@
       <c r="I18" s="10">
         <v>0</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="27">
         <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="8">
+        <v>100</v>
+      </c>
+      <c r="D19" s="9">
+        <v>75</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="27">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="8">
+        <v>100</v>
+      </c>
+      <c r="D20" s="9">
+        <v>100</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="27">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="34">
+        <v>100</v>
+      </c>
+      <c r="D21" s="35">
+        <v>75</v>
+      </c>
+      <c r="E21" s="35">
+        <v>0</v>
+      </c>
+      <c r="F21" s="35">
+        <v>0</v>
+      </c>
+      <c r="G21" s="35">
+        <v>0</v>
+      </c>
+      <c r="H21" s="35">
+        <v>0</v>
+      </c>
+      <c r="I21" s="36">
+        <v>0</v>
+      </c>
+      <c r="J21" s="28">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="11">
+        <f t="shared" ref="C22:J22" si="2">AVERAGE(C2:C21)</f>
+        <v>95.263157894736835</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="2"/>
+        <v>84.15789473684211</v>
+      </c>
+      <c r="E22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="22">
+        <f t="shared" si="2"/>
+        <v>17.942105263157895</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="23">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="8">
-        <v>100</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="10">
-        <v>0</v>
-      </c>
-      <c r="J19" s="29">
-        <f t="shared" si="1"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="24">
+        <v>60</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="24">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="8">
-        <v>100</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0</v>
-      </c>
-      <c r="I20" s="10">
-        <v>0</v>
-      </c>
-      <c r="J20" s="29">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="37">
-        <v>100</v>
-      </c>
-      <c r="D21" s="38">
-        <v>0</v>
-      </c>
-      <c r="E21" s="38">
-        <v>0</v>
-      </c>
-      <c r="F21" s="38">
-        <v>0</v>
-      </c>
-      <c r="G21" s="38">
-        <v>0</v>
-      </c>
-      <c r="H21" s="38">
-        <v>0</v>
-      </c>
-      <c r="I21" s="39">
-        <v>0</v>
-      </c>
-      <c r="J21" s="30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13">
-        <f t="shared" ref="C22:J22" si="2">AVERAGE(C2:C21)</f>
-        <v>95.25</v>
-      </c>
-      <c r="D22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="24">
-        <f t="shared" si="2"/>
-        <v>9.5250000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="25">
-        <v>10</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="26">
-        <v>60</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="26">
-        <v>10</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="24">
         <v>20</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="19">
         <v>-10</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="21">
+      <c r="B30" s="19">
         <v>-10</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="33"/>
-      <c r="J31" s="16"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="H31:I31"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J22">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
3. ödev not güncellemesi
Melike Yoğurtçu: 0->60
</commit_message>
<xml_diff>
--- a/notlar.xlsx
+++ b/notlar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.kasif\Desktop\workspace\Algorithms-and-Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet\Desktop\workspace\Algorithms-and-Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1469,7 +1469,7 @@
         <v>63</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1479,7 +1479,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="25">
         <f t="shared" si="1"/>
-        <v>44.666666666666671</v>
+        <v>54.666666666666664</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="E22" s="11">
         <f t="shared" si="2"/>
-        <v>75.421052631578945</v>
+        <v>78.578947368421055</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -1697,7 +1697,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="20">
         <f t="shared" si="2"/>
-        <v>80.94736842105263</v>
+        <v>81.473684210526315</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>